<commit_message>
bohr model with params
</commit_message>
<xml_diff>
--- a/UNIDADES.xlsx
+++ b/UNIDADES.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FCB9BDD9-AE3A-46CA-81C2-C84F52E0594F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="102">
   <si>
     <t>Comprimento</t>
   </si>
@@ -322,6 +323,9 @@
   </si>
   <si>
     <t>Nosso resultado</t>
+  </si>
+  <si>
+    <t>Calculo a partir da energia</t>
   </si>
 </sst>
 </file>
@@ -651,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:T100"/>
+  <dimension ref="C2:U100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D84" workbookViewId="0">
-      <selection activeCell="J102" sqref="J102"/>
+    <sheetView tabSelected="1" topLeftCell="D64" workbookViewId="0">
+      <selection activeCell="U70" sqref="U70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,12 +1420,12 @@
         <v>2724.8715280843912</v>
       </c>
     </row>
-    <row r="65" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J65" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J67" t="s">
         <v>68</v>
       </c>
@@ -1436,8 +1440,11 @@
         <f>K68/2</f>
         <v>0.25784960024410492</v>
       </c>
-    </row>
-    <row r="68" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="S67" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J68" t="s">
         <v>70</v>
       </c>
@@ -1451,13 +1458,26 @@
         <f>SQRT(3)*N67</f>
         <v>0.44660860833411409</v>
       </c>
-    </row>
-    <row r="69" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="S68" s="3"/>
+    </row>
+    <row r="69" spans="10:21" x14ac:dyDescent="0.25">
       <c r="N69">
         <v>0.95262794416288255</v>
       </c>
-    </row>
-    <row r="71" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="U69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="S70">
+        <f>(3-9*SQRT(3))/(12*SQRT(3)*U70)</f>
+        <v>0.51569920048821016</v>
+      </c>
+      <c r="U70">
+        <v>-1.17444904341371</v>
+      </c>
+    </row>
+    <row r="71" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J71" t="s">
         <v>69</v>
       </c>
@@ -1469,7 +1489,7 @@
         <v>1.5961143276988841</v>
       </c>
     </row>
-    <row r="72" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J72" t="s">
         <v>73</v>
       </c>
@@ -1477,8 +1497,12 @@
         <f>K71*K67</f>
         <v>1.621636624727925</v>
       </c>
-    </row>
-    <row r="74" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="S72">
+        <f>S70*SQRT(3)</f>
+        <v>0.89321721666822873</v>
+      </c>
+    </row>
+    <row r="74" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J74" t="s">
         <v>74</v>
       </c>
@@ -1486,8 +1510,12 @@
         <f>SQRT((9 - SQRT(3))/(12*K68))</f>
         <v>1.0837200023131948</v>
       </c>
-    </row>
-    <row r="77" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="S74">
+        <f>SQRT((9 - SQRT(3))/(12*S70))</f>
+        <v>1.0837200023131945</v>
+      </c>
+    </row>
+    <row r="77" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J77" t="s">
         <v>75</v>
       </c>
@@ -1502,7 +1530,7 @@
         <v>4.7469999999999999</v>
       </c>
     </row>
-    <row r="79" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J79" t="s">
         <v>83</v>
       </c>
@@ -1520,7 +1548,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="10:21" x14ac:dyDescent="0.25">
       <c r="M80" s="2" t="s">
         <v>81</v>
       </c>

</xml_diff>